<commit_message>
UPdating part for 10Amp fuse to more in-stock part
</commit_message>
<xml_diff>
--- a/Electrical/Electronics-pcb-rework-partslist.xlsx
+++ b/Electrical/Electronics-pcb-rework-partslist.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ejunkins\Desktop\open-source-rover\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ejunkins\Desktop\open-source-rover\Electrical\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="10785" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="10785"/>
   </bookViews>
   <sheets>
     <sheet name="Control Board" sheetId="1" r:id="rId1"/>
@@ -146,12 +146,6 @@
     <t xml:space="preserve">USB A Connector </t>
   </si>
   <si>
-    <t>https://www.digikey.com/product-detail/en/0697H9100-02/507-1937-1-ND/5208805/?itemSeq=281160146</t>
-  </si>
-  <si>
-    <t>507-1937-1-ND</t>
-  </si>
-  <si>
     <t>F1</t>
   </si>
   <si>
@@ -486,6 +480,12 @@
   </si>
   <si>
     <t>Suggested Qty to Buy</t>
+  </si>
+  <si>
+    <t>507-1916-ND</t>
+  </si>
+  <si>
+    <t>https://www.digikey.com/products/en?keywords=507-1916-ND</t>
   </si>
 </sst>
 </file>
@@ -928,8 +928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J55"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -944,39 +944,39 @@
   <sheetData>
     <row r="1" spans="1:10" ht="73.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="20" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I1" s="18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J1" s="18" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B2" s="4">
         <v>5</v>
@@ -991,10 +991,10 @@
         <v>37</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H2" s="3">
         <v>1.74</v>
@@ -1004,12 +1004,12 @@
         <v>8.6999999999999993</v>
       </c>
       <c r="J2" s="10" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B3" s="4">
         <v>10</v>
@@ -1024,10 +1024,10 @@
         <v>37</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H3" s="3">
         <v>1.24</v>
@@ -1037,12 +1037,12 @@
         <v>12.4</v>
       </c>
       <c r="J3" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B4" s="28">
         <v>3</v>
@@ -1057,10 +1057,10 @@
         <v>37</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="G4" s="13" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H4" s="17">
         <v>0.75</v>
@@ -1070,12 +1070,12 @@
         <v>2.25</v>
       </c>
       <c r="J4" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="14" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B5" s="28">
         <v>3</v>
@@ -1090,10 +1090,10 @@
         <v>37</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="G5" s="13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H5" s="3">
         <v>0.51</v>
@@ -1103,12 +1103,12 @@
         <v>1.53</v>
       </c>
       <c r="J5" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="14" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B6" s="28">
         <v>2</v>
@@ -1123,10 +1123,10 @@
         <v>37</v>
       </c>
       <c r="F6" s="14" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="G6" s="27" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H6" s="3">
         <v>0.33</v>
@@ -1136,12 +1136,12 @@
         <v>0.66</v>
       </c>
       <c r="J6" s="24" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B7" s="28">
         <v>7</v>
@@ -1156,10 +1156,10 @@
         <v>37</v>
       </c>
       <c r="F7" s="14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G7" s="13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H7" s="3">
         <v>0.49</v>
@@ -1169,12 +1169,12 @@
         <v>3.4299999999999997</v>
       </c>
       <c r="J7" s="10" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B8" s="28">
         <v>2</v>
@@ -1189,10 +1189,10 @@
         <v>37</v>
       </c>
       <c r="F8" s="14" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H8" s="3">
         <v>0.73</v>
@@ -1202,12 +1202,12 @@
         <v>1.46</v>
       </c>
       <c r="J8" s="10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" s="14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B9" s="28">
         <v>5</v>
@@ -1222,10 +1222,10 @@
         <v>37</v>
       </c>
       <c r="F9" s="14" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G9" s="13" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H9" s="3">
         <v>1.26</v>
@@ -1235,12 +1235,12 @@
         <v>6.3</v>
       </c>
       <c r="J9" s="10" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B10" s="4">
         <v>16</v>
@@ -1255,10 +1255,10 @@
         <v>37</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="G10" s="13" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H10" s="3">
         <v>0.182</v>
@@ -1268,12 +1268,12 @@
         <v>2.9119999999999999</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" s="14" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B11" s="28">
         <v>10</v>
@@ -1288,10 +1288,10 @@
         <v>37</v>
       </c>
       <c r="F11" s="14" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="G11" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H11" s="3">
         <v>4.1000000000000002E-2</v>
@@ -1301,12 +1301,12 @@
         <v>0.41000000000000003</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" s="14" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B12" s="28">
         <v>10</v>
@@ -1321,10 +1321,10 @@
         <v>37</v>
       </c>
       <c r="F12" s="14" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H12" s="3">
         <v>4.1000000000000002E-2</v>
@@ -1334,12 +1334,12 @@
         <v>0.41000000000000003</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" s="14" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B13" s="28">
         <v>10</v>
@@ -1354,10 +1354,10 @@
         <v>37</v>
       </c>
       <c r="F13" s="14" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H13" s="3">
         <v>4.1000000000000002E-2</v>
@@ -1367,12 +1367,12 @@
         <v>0.41000000000000003</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B14" s="4">
         <v>10</v>
@@ -1387,10 +1387,10 @@
         <v>37</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G14" s="16" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H14" s="15">
         <v>5.8999999999999997E-2</v>
@@ -1400,12 +1400,12 @@
         <v>0.59</v>
       </c>
       <c r="J14" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" s="14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B15" s="28">
         <v>2</v>
@@ -1420,10 +1420,10 @@
         <v>37</v>
       </c>
       <c r="F15" s="14" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H15" s="3">
         <v>0.45</v>
@@ -1433,12 +1433,12 @@
         <v>0.9</v>
       </c>
       <c r="J15" s="24" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A16" s="14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B16" s="28">
         <v>10</v>
@@ -1453,10 +1453,10 @@
         <v>37</v>
       </c>
       <c r="F16" s="14" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="G16" s="13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="H16" s="3">
         <v>0.17299999999999999</v>
@@ -1466,12 +1466,12 @@
         <v>1.73</v>
       </c>
       <c r="J16" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A17" s="14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B17" s="28">
         <v>1</v>
@@ -1486,10 +1486,10 @@
         <v>37</v>
       </c>
       <c r="F17" s="14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H17" s="3">
         <v>1.55</v>
@@ -1499,12 +1499,12 @@
         <v>1.55</v>
       </c>
       <c r="J17" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A18" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B18" s="28">
         <v>1</v>
@@ -1519,20 +1519,20 @@
         <v>37</v>
       </c>
       <c r="F18" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="G18" s="13" t="s">
-        <v>40</v>
+        <v>39</v>
+      </c>
+      <c r="G18" s="27" t="s">
+        <v>151</v>
       </c>
       <c r="H18" s="3">
-        <v>0.38</v>
+        <v>0.35</v>
       </c>
       <c r="I18" s="3">
         <f t="shared" si="0"/>
-        <v>0.38</v>
-      </c>
-      <c r="J18" s="10" t="s">
-        <v>39</v>
+        <v>0.35</v>
+      </c>
+      <c r="J18" s="24" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.45">
@@ -1552,7 +1552,7 @@
         <v>37</v>
       </c>
       <c r="F19" s="14" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="G19" s="13" t="s">
         <v>36</v>
@@ -1595,7 +1595,7 @@
     <row r="24" spans="1:10" x14ac:dyDescent="0.45">
       <c r="I24" s="1">
         <f>SUM(I2:I19)</f>
-        <v>47.021999999999991</v>
+        <v>46.99199999999999</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.45">
@@ -1737,9 +1737,9 @@
     <hyperlink ref="J16" r:id="rId9"/>
     <hyperlink ref="J19" r:id="rId10"/>
     <hyperlink ref="J17" r:id="rId11"/>
-    <hyperlink ref="J18" r:id="rId12"/>
-    <hyperlink ref="J15" r:id="rId13"/>
-    <hyperlink ref="J6" r:id="rId14"/>
+    <hyperlink ref="J15" r:id="rId12"/>
+    <hyperlink ref="J6" r:id="rId13"/>
+    <hyperlink ref="J18" r:id="rId14"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId15"/>
@@ -1750,7 +1750,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -1766,39 +1766,39 @@
   <sheetData>
     <row r="1" spans="1:10" ht="52.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="20" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="G1" s="18" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="I1" s="18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="J1" s="18" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A2" s="14" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B2" s="28">
         <v>1</v>
@@ -1813,10 +1813,10 @@
         <v>37</v>
       </c>
       <c r="F2" s="14" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G2" s="13" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H2" s="3">
         <v>0.48</v>
@@ -1826,12 +1826,12 @@
         <v>0.48</v>
       </c>
       <c r="J2" s="24" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="14" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B3" s="28">
         <v>2</v>
@@ -1846,10 +1846,10 @@
         <v>37</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="G3" s="13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H3" s="3">
         <v>0.51</v>
@@ -1859,12 +1859,12 @@
         <v>1.02</v>
       </c>
       <c r="J3" s="24" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A4" s="14" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B4" s="28">
         <v>1</v>
@@ -1879,10 +1879,10 @@
         <v>37</v>
       </c>
       <c r="F4" s="14" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H4" s="3">
         <v>0.42</v>
@@ -1892,12 +1892,12 @@
         <v>0.42</v>
       </c>
       <c r="J4" s="24" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="14" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="B5" s="28">
         <v>2</v>
@@ -1912,10 +1912,10 @@
         <v>37</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="G5" s="27" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H5" s="3">
         <v>0.33</v>
@@ -1925,7 +1925,7 @@
         <v>0.66</v>
       </c>
       <c r="J5" s="24" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
@@ -2441,36 +2441,36 @@
   <sheetData>
     <row r="1" spans="1:9" ht="73.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="20" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I1" s="18" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B2" s="4">
         <v>1</v>
@@ -2482,7 +2482,7 @@
         <v>1</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F2" s="4">
         <v>1988</v>
@@ -2491,16 +2491,16 @@
         <v>2.95</v>
       </c>
       <c r="H2" s="3">
-        <f>G2*B2</f>
+        <f t="shared" ref="H2:H18" si="0">G2*B2</f>
         <v>2.95</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A3" s="14" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B3" s="28">
         <v>1</v>
@@ -2515,22 +2515,22 @@
         <v>37</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G3" s="3">
         <v>1.4</v>
       </c>
       <c r="H3" s="3">
-        <f>G3*B3</f>
+        <f t="shared" si="0"/>
         <v>1.4</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="B4" s="4">
         <v>1</v>
@@ -2545,17 +2545,17 @@
         <v>37</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="G4" s="2">
         <v>1.55</v>
       </c>
       <c r="H4" s="3">
-        <f>G4*B4</f>
+        <f t="shared" si="0"/>
         <v>1.55</v>
       </c>
       <c r="I4" s="24" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
@@ -2575,17 +2575,17 @@
         <v>33</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="G5" s="3">
         <v>4.37</v>
       </c>
       <c r="H5" s="3">
-        <f>G5*B5</f>
+        <f t="shared" si="0"/>
         <v>4.37</v>
       </c>
       <c r="I5" s="24" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
@@ -2611,7 +2611,7 @@
         <v>0.45</v>
       </c>
       <c r="H6" s="3">
-        <f>G6*B6</f>
+        <f t="shared" si="0"/>
         <v>1.8</v>
       </c>
       <c r="I6" s="10" t="s">
@@ -2641,7 +2641,7 @@
         <v>0.27</v>
       </c>
       <c r="H7" s="3">
-        <f>G7*B7</f>
+        <f t="shared" si="0"/>
         <v>5.4</v>
       </c>
       <c r="I7" s="10" t="s">
@@ -2671,7 +2671,7 @@
         <v>0.41</v>
       </c>
       <c r="H8" s="3">
-        <f>G8*B8</f>
+        <f t="shared" si="0"/>
         <v>1.64</v>
       </c>
       <c r="I8" s="10" t="s">
@@ -2701,7 +2701,7 @@
         <v>0.59</v>
       </c>
       <c r="H9" s="3">
-        <f>G9*B9</f>
+        <f t="shared" si="0"/>
         <v>4.72</v>
       </c>
       <c r="I9" s="10" t="s">
@@ -2731,7 +2731,7 @@
         <v>3.78</v>
       </c>
       <c r="H10" s="3">
-        <f>G10*B10</f>
+        <f t="shared" si="0"/>
         <v>3.78</v>
       </c>
       <c r="I10" s="10" t="s">
@@ -2761,7 +2761,7 @@
         <v>3.02</v>
       </c>
       <c r="H11" s="3">
-        <f>G11*B11</f>
+        <f t="shared" si="0"/>
         <v>3.02</v>
       </c>
       <c r="I11" s="10" t="s">
@@ -2791,7 +2791,7 @@
         <v>3.72</v>
       </c>
       <c r="H12" s="3">
-        <f>G12*B12</f>
+        <f t="shared" si="0"/>
         <v>3.72</v>
       </c>
       <c r="I12" s="10" t="s">
@@ -2821,7 +2821,7 @@
         <v>7.07</v>
       </c>
       <c r="H13" s="3">
-        <f>G13*B13</f>
+        <f t="shared" si="0"/>
         <v>7.07</v>
       </c>
       <c r="I13" s="10" t="s">
@@ -2851,7 +2851,7 @@
         <v>9.9499999999999993</v>
       </c>
       <c r="H14" s="3">
-        <f>G14*B14</f>
+        <f t="shared" si="0"/>
         <v>9.9499999999999993</v>
       </c>
       <c r="I14" s="10" t="s">
@@ -2881,7 +2881,7 @@
         <v>14.95</v>
       </c>
       <c r="H15" s="7">
-        <f>G15*B15</f>
+        <f t="shared" si="0"/>
         <v>14.95</v>
       </c>
       <c r="I15" s="6" t="s">
@@ -2890,7 +2890,7 @@
     </row>
     <row r="16" spans="1:9" ht="13.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B16" s="4">
         <v>1</v>
@@ -2905,22 +2905,22 @@
         <v>37</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G16" s="3">
         <v>23.8</v>
       </c>
       <c r="H16" s="3">
-        <f>G16*B16</f>
+        <f t="shared" si="0"/>
         <v>23.8</v>
       </c>
       <c r="I16" s="24" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B17" s="4">
         <v>1</v>
@@ -2941,16 +2941,16 @@
         <v>35.68</v>
       </c>
       <c r="H17" s="3">
-        <f>G17*B17</f>
+        <f t="shared" si="0"/>
         <v>35.68</v>
       </c>
       <c r="I17" s="24" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B18" s="4">
         <v>5</v>
@@ -2971,11 +2971,11 @@
         <v>69.95</v>
       </c>
       <c r="H18" s="3">
-        <f>G18*B18</f>
+        <f t="shared" si="0"/>
         <v>349.75</v>
       </c>
       <c r="I18" s="24" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.45">
@@ -3150,36 +3150,36 @@
   <sheetData>
     <row r="1" spans="1:9" ht="52.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="20" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C1" s="20" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E1" s="18" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F1" s="18" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H1" s="18" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="I1" s="18" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="9" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B2" s="9">
         <v>1</v>
@@ -3202,12 +3202,12 @@
         <v>17.989999999999998</v>
       </c>
       <c r="I2" s="21" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="3" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" s="9" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B3" s="9">
         <v>1</v>
@@ -3230,12 +3230,12 @@
         <v>32.99</v>
       </c>
       <c r="I3" s="21" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="5" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" s="9" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B4" s="9">
         <v>5</v>
@@ -3250,7 +3250,7 @@
         <v>37</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G4" s="7">
         <v>2.46</v>
@@ -3260,7 +3260,7 @@
         <v>12.3</v>
       </c>
       <c r="I4" s="21" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Creating an initial assembly document about building the Control Board PCB. WIP
</commit_message>
<xml_diff>
--- a/Electrical/Electronics-pcb-rework-partslist.xlsx
+++ b/Electrical/Electronics-pcb-rework-partslist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="154">
   <si>
     <t>https://www.pololu.com/product/2851</t>
   </si>
@@ -419,9 +419,6 @@
     <t>J6-7</t>
   </si>
   <si>
-    <t>C2-17</t>
-  </si>
-  <si>
     <t>SuggestedQty to Buy</t>
   </si>
   <si>
@@ -486,6 +483,12 @@
   </si>
   <si>
     <t>https://www.digikey.com/products/en?keywords=507-1916-ND</t>
+  </si>
+  <si>
+    <t>Scematic Ref Des</t>
+  </si>
+  <si>
+    <t>C1-17</t>
   </si>
 </sst>
 </file>
@@ -926,28 +929,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J55"/>
+  <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="34.19921875" customWidth="1"/>
     <col min="2" max="2" width="12.9296875" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" customWidth="1"/>
-    <col min="8" max="9" width="18.33203125" customWidth="1"/>
-    <col min="10" max="10" width="63.19921875" customWidth="1"/>
+    <col min="7" max="7" width="14.6640625" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" customWidth="1"/>
+    <col min="9" max="10" width="18.33203125" customWidth="1"/>
+    <col min="11" max="11" width="63.19921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="73.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:11" ht="73.900000000000006" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A1" s="20" t="s">
         <v>108</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C1" s="20" t="s">
         <v>106</v>
@@ -958,23 +961,24 @@
       <c r="E1" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="F1" s="18" t="s">
-        <v>103</v>
-      </c>
-      <c r="G1" s="18" t="s">
+      <c r="F1" s="18"/>
+      <c r="G1" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="H1" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="I1" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="J1" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="K1" s="18" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>98</v>
       </c>
@@ -990,24 +994,25 @@
       <c r="E2" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="2"/>
+      <c r="G2" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="H2" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="H2" s="3">
+      <c r="I2" s="3">
         <v>1.74</v>
       </c>
-      <c r="I2" s="3">
-        <f t="shared" ref="I2:I19" si="0">H2*B2</f>
+      <c r="J2" s="3">
+        <f t="shared" ref="J2:J19" si="0">I2*B2</f>
         <v>8.6999999999999993</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="K2" s="10" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A3" s="2" t="s">
         <v>95</v>
       </c>
@@ -1023,24 +1028,25 @@
       <c r="E3" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="2"/>
+      <c r="G3" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="H3" s="13" t="s">
         <v>94</v>
       </c>
-      <c r="H3" s="3">
+      <c r="I3" s="3">
         <v>1.24</v>
       </c>
-      <c r="I3" s="3">
+      <c r="J3" s="3">
         <f t="shared" si="0"/>
         <v>12.4</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="K3" s="10" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="14" t="s">
         <v>92</v>
       </c>
@@ -1056,24 +1062,25 @@
       <c r="E4" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F4" s="14"/>
+      <c r="G4" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="G4" s="13" t="s">
+      <c r="H4" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="H4" s="17">
+      <c r="I4" s="17">
         <v>0.75</v>
       </c>
-      <c r="I4" s="3">
+      <c r="J4" s="3">
         <f t="shared" si="0"/>
         <v>2.25</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="K4" s="10" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="14" t="s">
         <v>88</v>
       </c>
@@ -1089,26 +1096,27 @@
       <c r="E5" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="G5" s="13" t="s">
+      <c r="F5" s="14"/>
+      <c r="G5" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="H5" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="H5" s="3">
+      <c r="I5" s="3">
         <v>0.51</v>
       </c>
-      <c r="I5" s="3">
+      <c r="J5" s="3">
         <f t="shared" si="0"/>
         <v>1.53</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="K5" s="10" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B6" s="28">
         <v>2</v>
@@ -1122,24 +1130,25 @@
       <c r="E6" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="14"/>
+      <c r="G6" s="14" t="s">
+        <v>142</v>
+      </c>
+      <c r="H6" s="27" t="s">
         <v>143</v>
       </c>
-      <c r="G6" s="27" t="s">
-        <v>144</v>
-      </c>
-      <c r="H6" s="3">
+      <c r="I6" s="3">
         <v>0.33</v>
       </c>
-      <c r="I6" s="3">
+      <c r="J6" s="3">
         <f t="shared" si="0"/>
         <v>0.66</v>
       </c>
-      <c r="J6" s="24" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K6" s="24" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="14" t="s">
         <v>85</v>
       </c>
@@ -1155,24 +1164,25 @@
       <c r="E7" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="14"/>
+      <c r="G7" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="H7" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="H7" s="3">
+      <c r="I7" s="3">
         <v>0.49</v>
       </c>
-      <c r="I7" s="3">
+      <c r="J7" s="3">
         <f t="shared" si="0"/>
         <v>3.4299999999999997</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="K7" s="10" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="14" t="s">
         <v>82</v>
       </c>
@@ -1188,24 +1198,25 @@
       <c r="E8" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="14"/>
+      <c r="G8" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="H8" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="H8" s="3">
+      <c r="I8" s="3">
         <v>0.73</v>
       </c>
-      <c r="I8" s="3">
+      <c r="J8" s="3">
         <f t="shared" si="0"/>
         <v>1.46</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="K8" s="10" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A9" s="14" t="s">
         <v>79</v>
       </c>
@@ -1221,29 +1232,30 @@
       <c r="E9" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="14"/>
+      <c r="G9" s="14" t="s">
         <v>78</v>
       </c>
-      <c r="G9" s="13" t="s">
+      <c r="H9" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="H9" s="3">
+      <c r="I9" s="3">
         <v>1.26</v>
       </c>
-      <c r="I9" s="3">
+      <c r="J9" s="3">
         <f t="shared" si="0"/>
         <v>6.3</v>
       </c>
-      <c r="J9" s="10" t="s">
+      <c r="K9" s="10" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A10" s="2" t="s">
         <v>75</v>
       </c>
       <c r="B10" s="4">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="C10" s="4">
         <v>16</v>
@@ -1254,24 +1266,25 @@
       <c r="E10" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="G10" s="13" t="s">
+      <c r="F10" s="2"/>
+      <c r="G10" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H10" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="H10" s="3">
+      <c r="I10" s="3">
         <v>0.182</v>
       </c>
-      <c r="I10" s="3">
+      <c r="J10" s="3">
         <f t="shared" si="0"/>
-        <v>2.9119999999999999</v>
-      </c>
-      <c r="J10" s="2" t="s">
+        <v>3.6399999999999997</v>
+      </c>
+      <c r="K10" s="24" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A11" s="14" t="s">
         <v>72</v>
       </c>
@@ -1287,24 +1300,25 @@
       <c r="E11" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="14"/>
+      <c r="G11" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="G11" s="13" t="s">
+      <c r="H11" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="H11" s="3">
+      <c r="I11" s="3">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="I11" s="3">
+      <c r="J11" s="3">
         <f t="shared" si="0"/>
         <v>0.41000000000000003</v>
       </c>
-      <c r="J11" s="2" t="s">
+      <c r="K11" s="24" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A12" s="14" t="s">
         <v>68</v>
       </c>
@@ -1320,24 +1334,25 @@
       <c r="E12" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="14"/>
+      <c r="G12" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="G12" s="13" t="s">
+      <c r="H12" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="H12" s="3">
+      <c r="I12" s="3">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="I12" s="3">
+      <c r="J12" s="3">
         <f t="shared" si="0"/>
         <v>0.41000000000000003</v>
       </c>
-      <c r="J12" s="2" t="s">
+      <c r="K12" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A13" s="14" t="s">
         <v>64</v>
       </c>
@@ -1353,24 +1368,25 @@
       <c r="E13" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="14"/>
+      <c r="G13" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="G13" s="13" t="s">
+      <c r="H13" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="H13" s="3">
+      <c r="I13" s="3">
         <v>4.1000000000000002E-2</v>
       </c>
-      <c r="I13" s="3">
+      <c r="J13" s="3">
         <f t="shared" si="0"/>
         <v>0.41000000000000003</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="K13" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A14" s="2" t="s">
         <v>60</v>
       </c>
@@ -1386,24 +1402,25 @@
       <c r="E14" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="2" t="s">
+      <c r="F14" s="2"/>
+      <c r="G14" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="G14" s="16" t="s">
+      <c r="H14" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="H14" s="15">
+      <c r="I14" s="15">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="I14" s="3">
+      <c r="J14" s="3">
         <f t="shared" si="0"/>
         <v>0.59</v>
       </c>
-      <c r="J14" s="10" t="s">
+      <c r="K14" s="10" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A15" s="14" t="s">
         <v>50</v>
       </c>
@@ -1419,24 +1436,25 @@
       <c r="E15" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="F15" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="G15" s="13" t="s">
+      <c r="F15" s="14"/>
+      <c r="G15" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="H15" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="H15" s="3">
+      <c r="I15" s="3">
         <v>0.45</v>
       </c>
-      <c r="I15" s="3">
+      <c r="J15" s="3">
         <f t="shared" si="0"/>
         <v>0.9</v>
       </c>
-      <c r="J15" s="24" t="s">
+      <c r="K15" s="24" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A16" s="14" t="s">
         <v>47</v>
       </c>
@@ -1452,24 +1470,25 @@
       <c r="E16" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="F16" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="G16" s="13" t="s">
+      <c r="F16" s="14"/>
+      <c r="G16" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="H16" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="H16" s="3">
+      <c r="I16" s="3">
         <v>0.17299999999999999</v>
       </c>
-      <c r="I16" s="3">
+      <c r="J16" s="3">
         <f t="shared" si="0"/>
         <v>1.73</v>
       </c>
-      <c r="J16" s="10" t="s">
+      <c r="K16" s="10" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A17" s="14" t="s">
         <v>44</v>
       </c>
@@ -1485,24 +1504,25 @@
       <c r="E17" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="F17" s="14" t="s">
+      <c r="F17" s="14"/>
+      <c r="G17" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="G17" s="13" t="s">
+      <c r="H17" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="H17" s="3">
+      <c r="I17" s="3">
         <v>1.55</v>
       </c>
-      <c r="I17" s="3">
+      <c r="J17" s="3">
         <f t="shared" si="0"/>
         <v>1.55</v>
       </c>
-      <c r="J17" s="10" t="s">
+      <c r="K17" s="10" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A18" s="14" t="s">
         <v>40</v>
       </c>
@@ -1518,24 +1538,25 @@
       <c r="E18" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="F18" s="14" t="s">
+      <c r="F18" s="14"/>
+      <c r="G18" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="G18" s="27" t="s">
-        <v>151</v>
-      </c>
-      <c r="H18" s="3">
+      <c r="H18" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="I18" s="3">
         <v>0.35</v>
       </c>
-      <c r="I18" s="3">
+      <c r="J18" s="3">
         <f t="shared" si="0"/>
         <v>0.35</v>
       </c>
-      <c r="J18" s="24" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="K18" s="24" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" s="14" t="s">
         <v>38</v>
       </c>
@@ -1551,198 +1572,203 @@
       <c r="E19" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="F19" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="G19" s="13" t="s">
+      <c r="F19" s="14"/>
+      <c r="G19" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="H19" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="H19" s="3">
+      <c r="I19" s="3">
         <v>0.5</v>
       </c>
-      <c r="I19" s="3">
+      <c r="J19" s="3">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="J19" s="10" t="s">
+      <c r="K19" s="10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="3"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="4"/>
       <c r="I20" s="3"/>
-      <c r="J20" s="2"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="J20" s="3"/>
+      <c r="K20" s="2"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="3"/>
+      <c r="G21" s="2"/>
+      <c r="H21" s="4"/>
       <c r="I21" s="3"/>
-      <c r="J21" s="2"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="I24" s="1">
-        <f>SUM(I2:I19)</f>
-        <v>46.99199999999999</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="H25" s="1"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="2"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.45">
+      <c r="J24" s="1">
+        <f>SUM(J2:J19)</f>
+        <v>47.719999999999992</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="H26" s="1"/>
+      <c r="K25" s="1"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.45">
       <c r="I26" s="1"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="H27" s="1"/>
+      <c r="J26" s="1"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.45">
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="H28" s="1"/>
+      <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="I28" s="1"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="H29" s="1"/>
+      <c r="J28" s="1"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="I29" s="1"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="H30" s="1"/>
+      <c r="J29" s="1"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="I30" s="1"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="H31" s="1"/>
+      <c r="J30" s="1"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="I31" s="1"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="H32" s="1"/>
+      <c r="J31" s="1"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="I32" s="1"/>
-    </row>
-    <row r="33" spans="8:9" x14ac:dyDescent="0.45">
-      <c r="H33" s="1"/>
+      <c r="J32" s="1"/>
+    </row>
+    <row r="33" spans="9:10" x14ac:dyDescent="0.45">
       <c r="I33" s="1"/>
-    </row>
-    <row r="34" spans="8:9" x14ac:dyDescent="0.45">
-      <c r="H34" s="1"/>
+      <c r="J33" s="1"/>
+    </row>
+    <row r="34" spans="9:10" x14ac:dyDescent="0.45">
       <c r="I34" s="1"/>
-    </row>
-    <row r="35" spans="8:9" x14ac:dyDescent="0.45">
-      <c r="H35" s="1"/>
+      <c r="J34" s="1"/>
+    </row>
+    <row r="35" spans="9:10" x14ac:dyDescent="0.45">
       <c r="I35" s="1"/>
-    </row>
-    <row r="36" spans="8:9" x14ac:dyDescent="0.45">
-      <c r="H36" s="1"/>
+      <c r="J35" s="1"/>
+    </row>
+    <row r="36" spans="9:10" x14ac:dyDescent="0.45">
       <c r="I36" s="1"/>
-    </row>
-    <row r="37" spans="8:9" x14ac:dyDescent="0.45">
-      <c r="H37" s="1"/>
+      <c r="J36" s="1"/>
+    </row>
+    <row r="37" spans="9:10" x14ac:dyDescent="0.45">
       <c r="I37" s="1"/>
-    </row>
-    <row r="38" spans="8:9" x14ac:dyDescent="0.45">
-      <c r="H38" s="1"/>
+      <c r="J37" s="1"/>
+    </row>
+    <row r="38" spans="9:10" x14ac:dyDescent="0.45">
       <c r="I38" s="1"/>
-    </row>
-    <row r="39" spans="8:9" x14ac:dyDescent="0.45">
-      <c r="H39" s="1"/>
+      <c r="J38" s="1"/>
+    </row>
+    <row r="39" spans="9:10" x14ac:dyDescent="0.45">
       <c r="I39" s="1"/>
-    </row>
-    <row r="40" spans="8:9" x14ac:dyDescent="0.45">
-      <c r="H40" s="1"/>
+      <c r="J39" s="1"/>
+    </row>
+    <row r="40" spans="9:10" x14ac:dyDescent="0.45">
       <c r="I40" s="1"/>
-    </row>
-    <row r="41" spans="8:9" x14ac:dyDescent="0.45">
-      <c r="H41" s="1"/>
+      <c r="J40" s="1"/>
+    </row>
+    <row r="41" spans="9:10" x14ac:dyDescent="0.45">
       <c r="I41" s="1"/>
-    </row>
-    <row r="42" spans="8:9" x14ac:dyDescent="0.45">
-      <c r="H42" s="1"/>
+      <c r="J41" s="1"/>
+    </row>
+    <row r="42" spans="9:10" x14ac:dyDescent="0.45">
       <c r="I42" s="1"/>
-    </row>
-    <row r="43" spans="8:9" x14ac:dyDescent="0.45">
-      <c r="H43" s="1"/>
+      <c r="J42" s="1"/>
+    </row>
+    <row r="43" spans="9:10" x14ac:dyDescent="0.45">
       <c r="I43" s="1"/>
-    </row>
-    <row r="44" spans="8:9" x14ac:dyDescent="0.45">
-      <c r="H44" s="1"/>
+      <c r="J43" s="1"/>
+    </row>
+    <row r="44" spans="9:10" x14ac:dyDescent="0.45">
       <c r="I44" s="1"/>
-    </row>
-    <row r="45" spans="8:9" x14ac:dyDescent="0.45">
-      <c r="H45" s="1"/>
+      <c r="J44" s="1"/>
+    </row>
+    <row r="45" spans="9:10" x14ac:dyDescent="0.45">
       <c r="I45" s="1"/>
-    </row>
-    <row r="46" spans="8:9" x14ac:dyDescent="0.45">
-      <c r="H46" s="1"/>
+      <c r="J45" s="1"/>
+    </row>
+    <row r="46" spans="9:10" x14ac:dyDescent="0.45">
       <c r="I46" s="1"/>
-    </row>
-    <row r="47" spans="8:9" x14ac:dyDescent="0.45">
-      <c r="H47" s="1"/>
+      <c r="J46" s="1"/>
+    </row>
+    <row r="47" spans="9:10" x14ac:dyDescent="0.45">
       <c r="I47" s="1"/>
-    </row>
-    <row r="48" spans="8:9" x14ac:dyDescent="0.45">
-      <c r="H48" s="1"/>
+      <c r="J47" s="1"/>
+    </row>
+    <row r="48" spans="9:10" x14ac:dyDescent="0.45">
       <c r="I48" s="1"/>
-    </row>
-    <row r="49" spans="8:9" x14ac:dyDescent="0.45">
-      <c r="H49" s="1"/>
+      <c r="J48" s="1"/>
+    </row>
+    <row r="49" spans="9:10" x14ac:dyDescent="0.45">
       <c r="I49" s="1"/>
-    </row>
-    <row r="50" spans="8:9" x14ac:dyDescent="0.45">
-      <c r="H50" s="1"/>
+      <c r="J49" s="1"/>
+    </row>
+    <row r="50" spans="9:10" x14ac:dyDescent="0.45">
       <c r="I50" s="1"/>
-    </row>
-    <row r="51" spans="8:9" x14ac:dyDescent="0.45">
-      <c r="H51" s="1"/>
+      <c r="J50" s="1"/>
+    </row>
+    <row r="51" spans="9:10" x14ac:dyDescent="0.45">
       <c r="I51" s="1"/>
-    </row>
-    <row r="52" spans="8:9" x14ac:dyDescent="0.45">
-      <c r="H52" s="1"/>
+      <c r="J51" s="1"/>
+    </row>
+    <row r="52" spans="9:10" x14ac:dyDescent="0.45">
       <c r="I52" s="1"/>
-    </row>
-    <row r="53" spans="8:9" x14ac:dyDescent="0.45">
-      <c r="H53" s="1"/>
+      <c r="J52" s="1"/>
+    </row>
+    <row r="53" spans="9:10" x14ac:dyDescent="0.45">
       <c r="I53" s="1"/>
-    </row>
-    <row r="54" spans="8:9" x14ac:dyDescent="0.45">
-      <c r="H54" s="1"/>
+      <c r="J53" s="1"/>
+    </row>
+    <row r="54" spans="9:10" x14ac:dyDescent="0.45">
       <c r="I54" s="1"/>
-    </row>
-    <row r="55" spans="8:9" x14ac:dyDescent="0.45">
-      <c r="H55" s="1"/>
+      <c r="J54" s="1"/>
+    </row>
+    <row r="55" spans="9:10" x14ac:dyDescent="0.45">
       <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1"/>
-    <hyperlink ref="J3" r:id="rId2"/>
-    <hyperlink ref="J4" r:id="rId3"/>
-    <hyperlink ref="J5" r:id="rId4"/>
-    <hyperlink ref="J7" r:id="rId5"/>
-    <hyperlink ref="J8" r:id="rId6"/>
-    <hyperlink ref="J9" r:id="rId7"/>
-    <hyperlink ref="J14" r:id="rId8"/>
-    <hyperlink ref="J16" r:id="rId9"/>
-    <hyperlink ref="J19" r:id="rId10"/>
-    <hyperlink ref="J17" r:id="rId11"/>
-    <hyperlink ref="J15" r:id="rId12"/>
-    <hyperlink ref="J6" r:id="rId13"/>
-    <hyperlink ref="J18" r:id="rId14"/>
+    <hyperlink ref="K2" r:id="rId1"/>
+    <hyperlink ref="K3" r:id="rId2"/>
+    <hyperlink ref="K4" r:id="rId3"/>
+    <hyperlink ref="K5" r:id="rId4"/>
+    <hyperlink ref="K7" r:id="rId5"/>
+    <hyperlink ref="K8" r:id="rId6"/>
+    <hyperlink ref="K9" r:id="rId7"/>
+    <hyperlink ref="K14" r:id="rId8"/>
+    <hyperlink ref="K16" r:id="rId9"/>
+    <hyperlink ref="K19" r:id="rId10"/>
+    <hyperlink ref="K17" r:id="rId11"/>
+    <hyperlink ref="K15" r:id="rId12"/>
+    <hyperlink ref="K6" r:id="rId13"/>
+    <hyperlink ref="K18" r:id="rId14"/>
+    <hyperlink ref="K10" r:id="rId15"/>
+    <hyperlink ref="K11" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId15"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
 </worksheet>
 </file>
 
@@ -1751,7 +1777,7 @@
   <dimension ref="A1:J73"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1769,7 +1795,7 @@
         <v>108</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C1" s="20" t="s">
         <v>106</v>
@@ -1846,7 +1872,7 @@
         <v>37</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G3" s="13" t="s">
         <v>87</v>
@@ -1897,7 +1923,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B5" s="28">
         <v>2</v>
@@ -1912,10 +1938,10 @@
         <v>37</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G5" s="27" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H5" s="3">
         <v>0.33</v>
@@ -1925,7 +1951,7 @@
         <v>0.66</v>
       </c>
       <c r="J5" s="24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
@@ -2425,7 +2451,7 @@
   <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2444,7 +2470,7 @@
         <v>108</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C1" s="20" t="s">
         <v>106</v>
@@ -2494,7 +2520,7 @@
         <f t="shared" ref="H2:H18" si="0">G2*B2</f>
         <v>2.95</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="24" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2530,7 +2556,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B4" s="4">
         <v>1</v>
@@ -2545,7 +2571,7 @@
         <v>37</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G4" s="2">
         <v>1.55</v>
@@ -2555,7 +2581,7 @@
         <v>1.55</v>
       </c>
       <c r="I4" s="24" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
@@ -2575,7 +2601,7 @@
         <v>33</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G5" s="3">
         <v>4.37</v>
@@ -2585,7 +2611,7 @@
         <v>4.37</v>
       </c>
       <c r="I5" s="24" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
@@ -2920,7 +2946,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B17" s="4">
         <v>1</v>
@@ -2945,12 +2971,12 @@
         <v>35.68</v>
       </c>
       <c r="I17" s="24" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B18" s="4">
         <v>5</v>
@@ -2975,7 +3001,7 @@
         <v>349.75</v>
       </c>
       <c r="I18" s="24" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.45">
@@ -3125,9 +3151,10 @@
     <hyperlink ref="I17" r:id="rId14"/>
     <hyperlink ref="I18" r:id="rId15"/>
     <hyperlink ref="I4" r:id="rId16"/>
+    <hyperlink ref="I2" r:id="rId17"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId17"/>
+  <pageSetup orientation="portrait" r:id="rId18"/>
 </worksheet>
 </file>
 
@@ -3136,7 +3163,7 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Adding the USB to TTL serial cable to the BOM of the electrical parts list
</commit_message>
<xml_diff>
--- a/Electrical/Electronics-pcb-rework-partslist.xlsx
+++ b/Electrical/Electronics-pcb-rework-partslist.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="10785"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22500" windowHeight="10785" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Control Board" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="156">
   <si>
     <t>https://www.pololu.com/product/2851</t>
   </si>
@@ -489,6 +489,12 @@
   </si>
   <si>
     <t>C1-17</t>
+  </si>
+  <si>
+    <t>USB to TTL Serial Adapter</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/JBtek-WINDOWS-Supported-Raspberry-Programming/dp/B00QT7LQ88/ref=sr_1_4?keywords=usb+to+ttl+serial+cable&amp;qid=1556583541&amp;s=gateway&amp;sr=8-4</t>
   </si>
 </sst>
 </file>
@@ -931,7 +937,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K55"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -2450,8 +2456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I51"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2517,7 +2523,7 @@
         <v>2.95</v>
       </c>
       <c r="H2" s="3">
-        <f t="shared" ref="H2:H18" si="0">G2*B2</f>
+        <f t="shared" ref="H2:H19" si="0">G2*B2</f>
         <v>2.95</v>
       </c>
       <c r="I2" s="24" t="s">
@@ -3002,6 +3008,36 @@
       </c>
       <c r="I18" s="24" t="s">
         <v>138</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A19" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="B19" s="4">
+        <v>1</v>
+      </c>
+      <c r="C19" s="4">
+        <v>1</v>
+      </c>
+      <c r="D19" s="4">
+        <v>1</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" t="s">
+        <v>9</v>
+      </c>
+      <c r="G19" s="3">
+        <v>6.99</v>
+      </c>
+      <c r="H19" s="3">
+        <f t="shared" si="0"/>
+        <v>6.99</v>
+      </c>
+      <c r="I19" s="24" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.45">
@@ -3012,8 +3048,8 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="G22" s="1"/>
       <c r="H22" s="1">
-        <f>SUM(H2:H18)</f>
-        <v>475.55</v>
+        <f>SUM(H2:H19)</f>
+        <v>482.54</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.45">
@@ -3152,9 +3188,10 @@
     <hyperlink ref="I18" r:id="rId15"/>
     <hyperlink ref="I4" r:id="rId16"/>
     <hyperlink ref="I2" r:id="rId17"/>
+    <hyperlink ref="I19" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId18"/>
+  <pageSetup orientation="portrait" r:id="rId19"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Changing USB cable to different part on amazon
</commit_message>
<xml_diff>
--- a/Electrical/Electronics-pcb-rework-partslist.xlsx
+++ b/Electrical/Electronics-pcb-rework-partslist.xlsx
@@ -428,9 +428,6 @@
     <t>J12,14</t>
   </si>
   <si>
-    <t>https://www.digikey.com/product-detail/en/tripp-lite/UR050-06N/TL1234-ND/5359410</t>
-  </si>
-  <si>
     <t>TL1234-ND</t>
   </si>
   <si>
@@ -495,6 +492,9 @@
   </si>
   <si>
     <t>https://www.amazon.com/JBtek-WINDOWS-Supported-Raspberry-Programming/dp/B00QT7LQ88/ref=sr_1_4?keywords=usb+to+ttl+serial+cable&amp;qid=1556583541&amp;s=gateway&amp;sr=8-4</t>
+  </si>
+  <si>
+    <t>https://www.amazon.com/gp/product/B00S8GU03A/ref=crt_ewc_img_dp_2?ie=UTF8&amp;psc=1&amp;smid=A1AMUYYA3CT6HJ</t>
   </si>
 </sst>
 </file>
@@ -969,7 +969,7 @@
       </c>
       <c r="F1" s="18"/>
       <c r="G1" s="20" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="H1" s="18" t="s">
         <v>102</v>
@@ -1104,7 +1104,7 @@
       </c>
       <c r="F5" s="14"/>
       <c r="G5" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="H5" s="13" t="s">
         <v>87</v>
@@ -1122,7 +1122,7 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B6" s="28">
         <v>2</v>
@@ -1138,10 +1138,10 @@
       </c>
       <c r="F6" s="14"/>
       <c r="G6" s="14" t="s">
+        <v>141</v>
+      </c>
+      <c r="H6" s="27" t="s">
         <v>142</v>
-      </c>
-      <c r="H6" s="27" t="s">
-        <v>143</v>
       </c>
       <c r="I6" s="3">
         <v>0.33</v>
@@ -1151,7 +1151,7 @@
         <v>0.66</v>
       </c>
       <c r="K6" s="24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.45">
@@ -1274,7 +1274,7 @@
       </c>
       <c r="F10" s="2"/>
       <c r="G10" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="H10" s="13" t="s">
         <v>74</v>
@@ -1549,7 +1549,7 @@
         <v>39</v>
       </c>
       <c r="H18" s="27" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="I18" s="3">
         <v>0.35</v>
@@ -1559,7 +1559,7 @@
         <v>0.35</v>
       </c>
       <c r="K18" s="24" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.45">
@@ -1801,7 +1801,7 @@
         <v>108</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C1" s="20" t="s">
         <v>106</v>
@@ -1878,7 +1878,7 @@
         <v>37</v>
       </c>
       <c r="F3" s="14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G3" s="13" t="s">
         <v>87</v>
@@ -1929,7 +1929,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A5" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B5" s="28">
         <v>2</v>
@@ -1944,10 +1944,10 @@
         <v>37</v>
       </c>
       <c r="F5" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G5" s="27" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="H5" s="3">
         <v>0.33</v>
@@ -1957,7 +1957,7 @@
         <v>0.66</v>
       </c>
       <c r="J5" s="24" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
@@ -2457,7 +2457,7 @@
   <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2562,7 +2562,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B4" s="4">
         <v>1</v>
@@ -2577,7 +2577,7 @@
         <v>37</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G4" s="2">
         <v>1.55</v>
@@ -2587,7 +2587,7 @@
         <v>1.55</v>
       </c>
       <c r="I4" s="24" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
@@ -2607,17 +2607,17 @@
         <v>33</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G5" s="3">
-        <v>4.37</v>
+        <v>7.99</v>
       </c>
       <c r="H5" s="3">
         <f t="shared" si="0"/>
-        <v>4.37</v>
+        <v>7.99</v>
       </c>
       <c r="I5" s="24" t="s">
-        <v>133</v>
+        <v>155</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
@@ -2952,7 +2952,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B17" s="4">
         <v>1</v>
@@ -2977,12 +2977,12 @@
         <v>35.68</v>
       </c>
       <c r="I17" s="24" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B18" s="4">
         <v>5</v>
@@ -3007,12 +3007,12 @@
         <v>349.75</v>
       </c>
       <c r="I18" s="24" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B19" s="4">
         <v>1</v>
@@ -3037,7 +3037,7 @@
         <v>6.99</v>
       </c>
       <c r="I19" s="24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.45">
@@ -3049,7 +3049,7 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1">
         <f>SUM(H2:H19)</f>
-        <v>482.54</v>
+        <v>486.16</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.45">
@@ -3182,13 +3182,13 @@
     <hyperlink ref="I11" r:id="rId9"/>
     <hyperlink ref="I12" r:id="rId10"/>
     <hyperlink ref="I13" r:id="rId11"/>
-    <hyperlink ref="I5" r:id="rId12"/>
-    <hyperlink ref="I16" r:id="rId13"/>
-    <hyperlink ref="I17" r:id="rId14"/>
-    <hyperlink ref="I18" r:id="rId15"/>
-    <hyperlink ref="I4" r:id="rId16"/>
-    <hyperlink ref="I2" r:id="rId17"/>
-    <hyperlink ref="I19" r:id="rId18"/>
+    <hyperlink ref="I16" r:id="rId12"/>
+    <hyperlink ref="I17" r:id="rId13"/>
+    <hyperlink ref="I18" r:id="rId14"/>
+    <hyperlink ref="I4" r:id="rId15"/>
+    <hyperlink ref="I2" r:id="rId16"/>
+    <hyperlink ref="I19" r:id="rId17"/>
+    <hyperlink ref="I5" r:id="rId18"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId19"/>

</xml_diff>

<commit_message>
Adding CAD files for head rework and pictures to put together
</commit_message>
<xml_diff>
--- a/Electrical/Electronics-pcb-rework-partslist.xlsx
+++ b/Electrical/Electronics-pcb-rework-partslist.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="159">
   <si>
     <t>https://www.pololu.com/product/2851</t>
   </si>
@@ -495,6 +495,15 @@
   </si>
   <si>
     <t>https://www.amazon.com/gp/product/B00S8GU03A/ref=crt_ewc_img_dp_2?ie=UTF8&amp;psc=1&amp;smid=A1AMUYYA3CT6HJ</t>
+  </si>
+  <si>
+    <t>https://www.mcmaster.com/90751a110</t>
+  </si>
+  <si>
+    <t>90751A110</t>
+  </si>
+  <si>
+    <t>M2.5 x 6 Screw</t>
   </si>
 </sst>
 </file>
@@ -2457,7 +2466,7 @@
   <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2523,7 +2532,7 @@
         <v>2.95</v>
       </c>
       <c r="H2" s="3">
-        <f t="shared" ref="H2:H19" si="0">G2*B2</f>
+        <f t="shared" ref="H2:H20" si="0">G2*B2</f>
         <v>2.95</v>
       </c>
       <c r="I2" s="24" t="s">
@@ -3038,6 +3047,36 @@
       </c>
       <c r="I19" s="24" t="s">
         <v>154</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A20" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B20" s="4">
+        <v>1</v>
+      </c>
+      <c r="C20" s="4">
+        <v>6</v>
+      </c>
+      <c r="D20" s="4">
+        <v>100</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F20" s="26" t="s">
+        <v>157</v>
+      </c>
+      <c r="G20" s="3">
+        <v>6.33</v>
+      </c>
+      <c r="H20" s="3">
+        <f t="shared" si="0"/>
+        <v>6.33</v>
+      </c>
+      <c r="I20" s="24" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.45">
@@ -3048,8 +3087,8 @@
     <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="G22" s="1"/>
       <c r="H22" s="1">
-        <f>SUM(H2:H19)</f>
-        <v>486.16</v>
+        <f>SUM(H2:H20)</f>
+        <v>492.49</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.45">
@@ -3189,9 +3228,10 @@
     <hyperlink ref="I2" r:id="rId16"/>
     <hyperlink ref="I19" r:id="rId17"/>
     <hyperlink ref="I5" r:id="rId18"/>
+    <hyperlink ref="I20" r:id="rId19"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId19"/>
+  <pageSetup orientation="portrait" r:id="rId20"/>
 </worksheet>
 </file>
 

</xml_diff>